<commit_message>
update bai tap assigment
</commit_message>
<xml_diff>
--- a/assignment/tran-thi-hang/assigment-webui/Data Files/excel-data/quan-ly-san-pham-gio-hang.xlsx
+++ b/assignment/tran-thi-hang/assigment-webui/Data Files/excel-data/quan-ly-san-pham-gio-hang.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>searchSanPham</t>
   </si>
@@ -33,16 +33,37 @@
   </si>
   <si>
     <t>productQuantity</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>hanghang@gmai.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
@@ -66,13 +87,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -351,37 +375,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>1234</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>